<commit_message>
Verify Feature #241: Min/max length enforced on text fields - PASSING
Feature #241 verification complete - all validation working correctly.

Test Coverage:
- Max length validation (Part Number: 50 chars, Notes: 500 chars)
- Min length validation (required fields: 1 char minimum)
- Valid length acceptance (all fields within acceptable ranges)
- Error message display (clear, red text, positioned correctly)
- Form state management (errors block submission, valid data proceeds)

Validation Framework:
- React Hook Form + Zod schemas
- Client-side validation working perfectly
- Error messages specific and actionable
- Zero JavaScript errors during testing

Results:
- All 8 test steps passed ✅
- 4 text fields tested (Part Number, Serial Number, Asset Name, Notes)
- 6 validation scenarios verified
- 4 screenshots captured for documentation

Progress: 240/374 features passing (64.2%)

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/.playwright-mcp/CUI-Sorties-20260120.xlsx
+++ b/.playwright-mcp/CUI-Sorties-20260120.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -426,12 +426,12 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Generated: 2026-01-20 04:36:42Z</v>
+        <v>Generated: 2026-01-20 09:56:08Z</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Total Sorties: 5</v>
+        <v>Total Sorties: 4</v>
       </c>
     </row>
     <row r="7">
@@ -468,115 +468,115 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>TEST-FEATURE-139-SORTIE</v>
+        <v>CRIIS-SORTIE-004</v>
       </c>
       <c r="B8" t="str">
-        <v>CRIIS-002</v>
+        <v>CRIIS-003</v>
       </c>
       <c r="C8" t="str">
-        <v>CRIIS-002</v>
+        <v>AC-003</v>
       </c>
       <c r="D8" t="str">
-        <v>2026-01-20 00:00:00Z</v>
+        <v>2026-01-18 00:00:00Z</v>
       </c>
       <c r="E8" t="str">
-        <v>Partial Mission Capable</v>
+        <v>Full Mission Capable</v>
       </c>
       <c r="F8" t="str">
-        <v/>
+        <v>Range C</v>
       </c>
       <c r="G8" t="str">
-        <v>CRIIS</v>
+        <v>Unit Charlie</v>
       </c>
       <c r="H8" t="str">
-        <v>CRIIS</v>
+        <v>Unit Charlie</v>
       </c>
       <c r="I8" t="str">
-        <v/>
+        <v>Surveillance mission</v>
       </c>
       <c r="J8" t="str">
-        <v/>
+        <v>All systems operational</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>CRIIS-SORTIE-004</v>
+        <v>CRIIS-SORTIE-002</v>
       </c>
       <c r="B9" t="str">
-        <v>CRIIS-003</v>
+        <v>CRIIS-005</v>
       </c>
       <c r="C9" t="str">
-        <v>AC-003</v>
+        <v>AC-005</v>
       </c>
       <c r="D9" t="str">
-        <v>2026-01-18 00:00:00Z</v>
+        <v>2026-01-17 00:00:00Z</v>
       </c>
       <c r="E9" t="str">
-        <v>Full Mission Capable</v>
+        <v>Partial Mission Capable</v>
       </c>
       <c r="F9" t="str">
-        <v>Range C</v>
+        <v>Range B</v>
       </c>
       <c r="G9" t="str">
-        <v>Unit Charlie</v>
+        <v>Unit Bravo</v>
       </c>
       <c r="H9" t="str">
-        <v>Unit Charlie</v>
+        <v>Unit Alpha</v>
       </c>
       <c r="I9" t="str">
-        <v>Surveillance mission</v>
+        <v>Training exercise</v>
       </c>
       <c r="J9" t="str">
-        <v>All systems operational</v>
+        <v>Camera system showed intermittent issues</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>CRIIS-SORTIE-002</v>
+        <v>CRIIS-SORTIE-001</v>
       </c>
       <c r="B10" t="str">
-        <v>CRIIS-005</v>
+        <v>CRIIS-001</v>
       </c>
       <c r="C10" t="str">
-        <v>AC-005</v>
+        <v>AC-001</v>
       </c>
       <c r="D10" t="str">
-        <v>2026-01-17 00:00:00Z</v>
+        <v>2026-01-15 00:00:00Z</v>
       </c>
       <c r="E10" t="str">
-        <v>Partial Mission Capable</v>
+        <v>Full Mission Capable</v>
       </c>
       <c r="F10" t="str">
-        <v>Range B</v>
+        <v>Range A</v>
       </c>
       <c r="G10" t="str">
-        <v>Unit Bravo</v>
+        <v>Unit Alpha</v>
       </c>
       <c r="H10" t="str">
         <v>Unit Alpha</v>
       </c>
       <c r="I10" t="str">
-        <v>Training exercise</v>
+        <v>Operational deployment</v>
       </c>
       <c r="J10" t="str">
-        <v>Camera system showed intermittent issues</v>
+        <v>Successful reconnaissance mission</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>CRIIS-SORTIE-001</v>
+        <v>CRIIS-SORTIE-003</v>
       </c>
       <c r="B11" t="str">
-        <v>CRIIS-001</v>
+        <v>CRIIS-006</v>
       </c>
       <c r="C11" t="str">
-        <v>AC-001</v>
+        <v>AC-006</v>
       </c>
       <c r="D11" t="str">
-        <v>2026-01-15 00:00:00Z</v>
+        <v>2026-01-10 00:00:00Z</v>
       </c>
       <c r="E11" t="str">
-        <v>Full Mission Capable</v>
+        <v>Non-Mission Capable</v>
       </c>
       <c r="F11" t="str">
         <v>Range A</v>
@@ -588,46 +588,14 @@
         <v>Unit Alpha</v>
       </c>
       <c r="I11" t="str">
-        <v>Operational deployment</v>
+        <v>Maintenance check flight</v>
       </c>
       <c r="J11" t="str">
-        <v>Successful reconnaissance mission</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>CRIIS-SORTIE-003</v>
-      </c>
-      <c r="B12" t="str">
-        <v>CRIIS-006</v>
-      </c>
-      <c r="C12" t="str">
-        <v>AC-006</v>
-      </c>
-      <c r="D12" t="str">
-        <v>2026-01-10 00:00:00Z</v>
-      </c>
-      <c r="E12" t="str">
-        <v>Non-Mission Capable</v>
-      </c>
-      <c r="F12" t="str">
-        <v>Range A</v>
-      </c>
-      <c r="G12" t="str">
-        <v>Unit Alpha</v>
-      </c>
-      <c r="H12" t="str">
-        <v>Unit Alpha</v>
-      </c>
-      <c r="I12" t="str">
-        <v>Maintenance check flight</v>
-      </c>
-      <c r="J12" t="str">
         <v>Power supply failure detected during flight</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="str">
+    <row r="13">
+      <c r="A13" t="str">
         <v>CUI - CONTROLLED UNCLASSIFIED INFORMATION</v>
       </c>
     </row>
@@ -637,10 +605,10 @@
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A4:J4"/>
     <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A14:J14"/>
+    <mergeCell ref="A13:J13"/>
   </mergeCells>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>